<commit_message>
Commiting the updated changes on 11-Dec-2023
</commit_message>
<xml_diff>
--- a/src/test/java/com/demoBankingV1/testData/LoginData.xlsx
+++ b/src/test/java/com/demoBankingV1/testData/LoginData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mtali\eclipse-workspace\demoBankingV1\src\test\java\com\demoBankingV1\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85EF772C-D641-41CD-922D-FCA4E92FFB7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828B1788-B712-436B-BA6A-B807614AA406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>Username</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>uzApegu</t>
+  </si>
+  <si>
+    <t>sEvYmEq</t>
+  </si>
+  <si>
+    <t>mngr601962</t>
   </si>
 </sst>
 </file>
@@ -358,7 +364,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A2" sqref="A2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -378,26 +384,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>